<commit_message>
update to new files
</commit_message>
<xml_diff>
--- a/working/armbruster/ON.ME.high.xlsx
+++ b/working/armbruster/ON.ME.high.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorjaelliott/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorjaelliott/Desktop/Repositories/LCAdata/working/armbruster/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{451271F7-28FA-7C4D-AF7F-70C70148DDAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76530AED-B757-C44B-BA81-10C1098B15C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7180" yWindow="4300" windowWidth="21620" windowHeight="12280" xr2:uid="{EDAB82BB-ACB3-8742-88AF-AE0EAD92E4E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>cross</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>F2</t>
+  </si>
+  <si>
+    <t>U</t>
   </si>
 </sst>
 </file>
@@ -423,7 +426,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D2" sqref="D2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,6 +464,18 @@
       <c r="C2">
         <v>9.5419847328244278E-3</v>
       </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -472,6 +487,18 @@
       <c r="C3">
         <v>1.1259541984732823E-2</v>
       </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -483,6 +510,18 @@
       <c r="C4">
         <v>4.7709923664122139E-3</v>
       </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -493,6 +532,18 @@
       </c>
       <c r="C5">
         <v>8.7786259541984737E-3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>